<commit_message>
species table and gene expression table modified
</commit_message>
<xml_diff>
--- a/Species_table.xlsx
+++ b/Species_table.xlsx
@@ -513,9 +513,6 @@
     <t>https://data.jgi.doe.gov/refine-download/phytozome?genome_id=677</t>
   </si>
   <si>
-    <t>http://ftp.ensemblgenomes.org/pub/plants/release-52/fasta/hordeum_vulgare/</t>
-  </si>
-  <si>
     <t>http://ftp.ensemblgenomes.org/pub/plants/release-53/fasta/actinidia_chinensis/</t>
   </si>
   <si>
@@ -646,6 +643,9 @@
   </si>
   <si>
     <t>https://data.jgi.doe.gov/refine-download/phytozome?genome_id=491</t>
+  </si>
+  <si>
+    <t>http://ftp.ensemblgenomes.org/pub/plants/release-51/fasta/hordeum_vulgare/</t>
   </si>
 </sst>
 </file>
@@ -1197,7 +1197,7 @@
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1233,7 +1233,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1253,7 +1253,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1273,7 +1273,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1293,7 +1293,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1313,7 +1313,7 @@
         <v>19</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1333,7 +1333,7 @@
         <v>22</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1367,7 +1367,7 @@
         <v>25</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1435,7 +1435,7 @@
         <v>31</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1455,7 +1455,7 @@
         <v>34</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1475,7 +1475,7 @@
         <v>37</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1495,7 +1495,7 @@
         <v>40</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1515,7 +1515,7 @@
         <v>43</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1535,7 +1535,7 @@
         <v>46</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1555,7 +1555,7 @@
         <v>49</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1592,7 +1592,7 @@
         <v>52</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1612,7 +1612,7 @@
         <v>55</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1632,7 +1632,7 @@
         <v>58</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1652,7 +1652,7 @@
         <v>61</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>163</v>
+        <v>207</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1672,7 +1672,7 @@
         <v>64</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1692,7 +1692,7 @@
         <v>67</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1712,7 +1712,7 @@
         <v>70</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1732,7 +1732,7 @@
         <v>73</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1752,7 +1752,7 @@
         <v>76</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1772,7 +1772,7 @@
         <v>79</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1792,7 +1792,7 @@
         <v>82</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1812,7 +1812,7 @@
         <v>85</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1832,7 +1832,7 @@
         <v>88</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1852,7 +1852,7 @@
         <v>91</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1872,7 +1872,7 @@
         <v>95</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1892,7 +1892,7 @@
         <v>98</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1912,7 +1912,7 @@
         <v>101</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1932,7 +1932,7 @@
         <v>104</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1952,7 +1952,7 @@
         <v>107</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1972,7 +1972,7 @@
         <v>110</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1992,7 +1992,7 @@
         <v>113</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2012,7 +2012,7 @@
         <v>116</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2032,7 +2032,7 @@
         <v>119</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2052,7 +2052,7 @@
         <v>122</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2090,7 +2090,7 @@
         <v>127</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2110,7 +2110,7 @@
         <v>130</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2130,7 +2130,7 @@
         <v>133</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2150,7 +2150,7 @@
         <v>136</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2170,7 +2170,7 @@
         <v>139</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2190,7 +2190,7 @@
         <v>142</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2210,7 +2210,7 @@
         <v>145</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
H. vulgare genome version in Species table changed
</commit_message>
<xml_diff>
--- a/Species_table.xlsx
+++ b/Species_table.xlsx
@@ -204,9 +204,6 @@
     <t>Hordeum vulgare</t>
   </si>
   <si>
-    <t>MorexV3_pseudomolecules_assembly</t>
-  </si>
-  <si>
     <t>GCA_904849725.1</t>
   </si>
   <si>
@@ -646,6 +643,9 @@
   </si>
   <si>
     <t>http://ftp.ensemblgenomes.org/pub/plants/release-51/fasta/hordeum_vulgare/</t>
+  </si>
+  <si>
+    <t>IBSV v2</t>
   </si>
 </sst>
 </file>
@@ -1196,8 +1196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1233,7 +1233,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1253,7 +1253,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1273,7 +1273,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1293,7 +1293,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1313,7 +1313,7 @@
         <v>19</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1333,12 +1333,12 @@
         <v>22</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -1347,7 +1347,7 @@
         <v>15368</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1367,12 +1367,12 @@
         <v>25</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -1381,12 +1381,12 @@
         <v>3711</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -1395,7 +1395,7 @@
         <v>90675</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1415,7 +1415,7 @@
         <v>28</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1435,7 +1435,7 @@
         <v>31</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1455,7 +1455,7 @@
         <v>34</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1475,7 +1475,7 @@
         <v>37</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1495,7 +1495,7 @@
         <v>40</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1515,7 +1515,7 @@
         <v>43</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1535,7 +1535,7 @@
         <v>46</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1555,12 +1555,12 @@
         <v>49</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
@@ -1569,10 +1569,10 @@
         <v>57918</v>
       </c>
       <c r="D19" t="s">
+        <v>160</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>161</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1592,7 +1592,7 @@
         <v>52</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1612,7 +1612,7 @@
         <v>55</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1632,7 +1632,7 @@
         <v>58</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1646,18 +1646,18 @@
         <v>112509</v>
       </c>
       <c r="D23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E23" t="s">
         <v>60</v>
       </c>
-      <c r="E23" t="s">
-        <v>61</v>
-      </c>
       <c r="F23" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
@@ -1666,18 +1666,18 @@
         <v>35885</v>
       </c>
       <c r="D24" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" t="s">
         <v>63</v>
       </c>
-      <c r="E24" t="s">
-        <v>64</v>
-      </c>
       <c r="F24" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B25" t="s">
         <v>6</v>
@@ -1686,18 +1686,18 @@
         <v>51240</v>
       </c>
       <c r="D25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" t="s">
         <v>66</v>
       </c>
-      <c r="E25" t="s">
-        <v>67</v>
-      </c>
       <c r="F25" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
         <v>6</v>
@@ -1706,18 +1706,18 @@
         <v>63787</v>
       </c>
       <c r="D26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" t="s">
         <v>69</v>
       </c>
-      <c r="E26" t="s">
-        <v>70</v>
-      </c>
       <c r="F26" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B27" t="s">
         <v>6</v>
@@ -1726,18 +1726,18 @@
         <v>4236</v>
       </c>
       <c r="D27" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" t="s">
         <v>72</v>
       </c>
-      <c r="E27" t="s">
-        <v>73</v>
-      </c>
       <c r="F27" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B28" t="s">
         <v>6</v>
@@ -1746,18 +1746,18 @@
         <v>3871</v>
       </c>
       <c r="D28" t="s">
+        <v>74</v>
+      </c>
+      <c r="E28" t="s">
         <v>75</v>
       </c>
-      <c r="E28" t="s">
-        <v>76</v>
-      </c>
       <c r="F28" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
@@ -1766,18 +1766,18 @@
         <v>3750</v>
       </c>
       <c r="D29" t="s">
+        <v>77</v>
+      </c>
+      <c r="E29" t="s">
         <v>78</v>
       </c>
-      <c r="E29" t="s">
-        <v>79</v>
-      </c>
       <c r="F29" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B30" t="s">
         <v>6</v>
@@ -1786,18 +1786,18 @@
         <v>3983</v>
       </c>
       <c r="D30" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30" t="s">
         <v>81</v>
       </c>
-      <c r="E30" t="s">
-        <v>82</v>
-      </c>
       <c r="F30" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B31" t="s">
         <v>6</v>
@@ -1806,18 +1806,18 @@
         <v>3880</v>
       </c>
       <c r="D31" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31" t="s">
         <v>84</v>
       </c>
-      <c r="E31" t="s">
-        <v>85</v>
-      </c>
       <c r="F31" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B32" t="s">
         <v>14</v>
@@ -1826,18 +1826,18 @@
         <v>214687</v>
       </c>
       <c r="D32" t="s">
+        <v>86</v>
+      </c>
+      <c r="E32" t="s">
         <v>87</v>
       </c>
-      <c r="E32" t="s">
-        <v>88</v>
-      </c>
       <c r="F32" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B33" t="s">
         <v>6</v>
@@ -1846,38 +1846,38 @@
         <v>49451</v>
       </c>
       <c r="D33" t="s">
+        <v>89</v>
+      </c>
+      <c r="E33" t="s">
         <v>90</v>
       </c>
-      <c r="E33" t="s">
-        <v>91</v>
-      </c>
       <c r="F33" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" t="s">
         <v>92</v>
-      </c>
-      <c r="B34" t="s">
-        <v>93</v>
       </c>
       <c r="C34">
         <v>210225</v>
       </c>
       <c r="D34" t="s">
+        <v>93</v>
+      </c>
+      <c r="E34" t="s">
         <v>94</v>
       </c>
-      <c r="E34" t="s">
-        <v>95</v>
-      </c>
       <c r="F34" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B35" t="s">
         <v>6</v>
@@ -1886,18 +1886,18 @@
         <v>158383</v>
       </c>
       <c r="D35" t="s">
+        <v>96</v>
+      </c>
+      <c r="E35" t="s">
         <v>97</v>
       </c>
-      <c r="E35" t="s">
-        <v>98</v>
-      </c>
       <c r="F35" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B36" t="s">
         <v>14</v>
@@ -1906,38 +1906,38 @@
         <v>39947</v>
       </c>
       <c r="D36" t="s">
+        <v>99</v>
+      </c>
+      <c r="E36" t="s">
         <v>100</v>
       </c>
-      <c r="E36" t="s">
-        <v>101</v>
-      </c>
       <c r="F36" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B37" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C37">
         <v>3469</v>
       </c>
       <c r="D37" t="s">
+        <v>102</v>
+      </c>
+      <c r="E37" t="s">
         <v>103</v>
       </c>
-      <c r="E37" t="s">
-        <v>104</v>
-      </c>
       <c r="F37" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B38" t="s">
         <v>6</v>
@@ -1946,18 +1946,18 @@
         <v>3885</v>
       </c>
       <c r="D38" t="s">
+        <v>105</v>
+      </c>
+      <c r="E38" t="s">
         <v>106</v>
       </c>
-      <c r="E38" t="s">
-        <v>107</v>
-      </c>
       <c r="F38" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B39" t="s">
         <v>6</v>
@@ -1966,18 +1966,18 @@
         <v>3694</v>
       </c>
       <c r="D39" t="s">
+        <v>108</v>
+      </c>
+      <c r="E39" t="s">
         <v>109</v>
       </c>
-      <c r="E39" t="s">
-        <v>110</v>
-      </c>
       <c r="F39" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B40" t="s">
         <v>6</v>
@@ -1986,18 +1986,18 @@
         <v>3760</v>
       </c>
       <c r="D40" t="s">
+        <v>111</v>
+      </c>
+      <c r="E40" t="s">
         <v>112</v>
       </c>
-      <c r="E40" t="s">
-        <v>113</v>
-      </c>
       <c r="F40" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B41" t="s">
         <v>6</v>
@@ -2006,18 +2006,18 @@
         <v>97700</v>
       </c>
       <c r="D41" t="s">
+        <v>114</v>
+      </c>
+      <c r="E41" t="s">
         <v>115</v>
       </c>
-      <c r="E41" t="s">
-        <v>116</v>
-      </c>
       <c r="F41" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B42" t="s">
         <v>6</v>
@@ -2026,18 +2026,18 @@
         <v>74649</v>
       </c>
       <c r="D42" t="s">
+        <v>117</v>
+      </c>
+      <c r="E42" t="s">
         <v>118</v>
       </c>
-      <c r="E42" t="s">
-        <v>119</v>
-      </c>
       <c r="F42" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B43" t="s">
         <v>6</v>
@@ -2046,18 +2046,18 @@
         <v>4182</v>
       </c>
       <c r="D43" t="s">
+        <v>120</v>
+      </c>
+      <c r="E43" t="s">
         <v>121</v>
       </c>
-      <c r="E43" t="s">
-        <v>122</v>
-      </c>
       <c r="F43" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B44" t="s">
         <v>6</v>
@@ -2066,16 +2066,16 @@
         <v>4081</v>
       </c>
       <c r="D44" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B45" t="s">
         <v>6</v>
@@ -2084,18 +2084,18 @@
         <v>4113</v>
       </c>
       <c r="D45" t="s">
+        <v>125</v>
+      </c>
+      <c r="E45" t="s">
         <v>126</v>
       </c>
-      <c r="E45" t="s">
-        <v>127</v>
-      </c>
       <c r="F45" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B46" t="s">
         <v>14</v>
@@ -2104,18 +2104,18 @@
         <v>4558</v>
       </c>
       <c r="D46" t="s">
+        <v>128</v>
+      </c>
+      <c r="E46" t="s">
         <v>129</v>
       </c>
-      <c r="E46" t="s">
-        <v>130</v>
-      </c>
       <c r="F46" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B47" t="s">
         <v>6</v>
@@ -2124,18 +2124,18 @@
         <v>3641</v>
       </c>
       <c r="D47" t="s">
+        <v>131</v>
+      </c>
+      <c r="E47" t="s">
         <v>132</v>
       </c>
-      <c r="E47" t="s">
-        <v>133</v>
-      </c>
       <c r="F47" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B48" t="s">
         <v>14</v>
@@ -2144,18 +2144,18 @@
         <v>4565</v>
       </c>
       <c r="D48" t="s">
+        <v>134</v>
+      </c>
+      <c r="E48" t="s">
         <v>135</v>
       </c>
-      <c r="E48" t="s">
-        <v>136</v>
-      </c>
       <c r="F48" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B49" t="s">
         <v>6</v>
@@ -2164,18 +2164,18 @@
         <v>3916</v>
       </c>
       <c r="D49" t="s">
+        <v>137</v>
+      </c>
+      <c r="E49" t="s">
         <v>138</v>
       </c>
-      <c r="E49" t="s">
-        <v>139</v>
-      </c>
       <c r="F49" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B50" t="s">
         <v>6</v>
@@ -2184,18 +2184,18 @@
         <v>29760</v>
       </c>
       <c r="D50" t="s">
+        <v>140</v>
+      </c>
+      <c r="E50" t="s">
         <v>141</v>
       </c>
-      <c r="E50" t="s">
-        <v>142</v>
-      </c>
       <c r="F50" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B51" t="s">
         <v>14</v>
@@ -2204,18 +2204,18 @@
         <v>4577</v>
       </c>
       <c r="D51" t="s">
+        <v>143</v>
+      </c>
+      <c r="E51" t="s">
         <v>144</v>
       </c>
-      <c r="E51" t="s">
-        <v>145</v>
-      </c>
       <c r="F51" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B52" t="s">
         <v>14</v>
@@ -2224,12 +2224,12 @@
         <v>78828</v>
       </c>
       <c r="F52" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B53" t="s">
         <v>6</v>
@@ -2238,12 +2238,12 @@
         <v>62330</v>
       </c>
       <c r="F53" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B54" t="s">
         <v>6</v>
@@ -2252,7 +2252,7 @@
         <v>3617</v>
       </c>
       <c r="F54" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>